<commit_message>
Add final result excel
</commit_message>
<xml_diff>
--- a/final_experiement_result.xlsx
+++ b/final_experiement_result.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckato\Documents\카카오톡 받은 파일\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckato\PycharmProjects\SentimentAnalysis_korean_GC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B2684F-878A-4FE6-B9A8-E6D881CA1BD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0736C71-438C-460E-944D-7B9FD7093DD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F17547EF-9B64-471A-BF66-AECF6CD11A8B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="30">
   <si>
     <t>model</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -148,6 +148,10 @@
   </si>
   <si>
     <t>SENTIMENT_ATT_LSTM_ATT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>att</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -517,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0417DA5-AD98-4B76-AFA2-00B2CD3D5F89}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -580,6 +584,9 @@
       <c r="A2" t="s">
         <v>20</v>
       </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
       <c r="C2" t="s">
         <v>13</v>
       </c>

</xml_diff>